<commit_message>
Update files for processing authors' folders
</commit_message>
<xml_diff>
--- a/Datasets_Processing/Authors_Gdocs.xlsx
+++ b/Datasets_Processing/Authors_Gdocs.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="391">
   <si>
     <t xml:space="preserve">Study ID</t>
   </si>
@@ -772,7 +772,7 @@
     <t xml:space="preserve">Jessica D. Petersen</t>
   </si>
   <si>
-    <t xml:space="preserve">jessica.petersen@cornell.edu</t>
+    <t xml:space="preserve">jessica.petersen@cornell.edu,jessica.d.petersen@state.mn.us</t>
   </si>
   <si>
     <t xml:space="preserve">Brian A. Nault</t>
@@ -1177,7 +1177,7 @@
     <t xml:space="preserve">Bryony Willcox</t>
   </si>
   <si>
-    <t xml:space="preserve">bwillcox@myune.edu.au</t>
+    <t xml:space="preserve">bwillcox@myune.edu.au,b.k.willcox@reading.ac.uk</t>
   </si>
   <si>
     <t xml:space="preserve">Yi_Zou_Brassica_napus_China_2015</t>
@@ -1235,13 +1235,28 @@
     <t xml:space="preserve">David Alomar</t>
   </si>
   <si>
-    <t xml:space="preserve">Co-author/Co-owner/Co-owner</t>
-  </si>
-  <si>
     <t xml:space="preserve">Miguel A. González-Estévez</t>
   </si>
   <si>
     <t xml:space="preserve">Amparo_Lázaro_Prunus_dulcis_2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katrine_Hansen_Psidium_guajava_Thailand_several_years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katrine Hansen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">katrinekvj@gmail.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuanjit Sritongchuay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benno I. Simmons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bo Dalsgaard</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1267,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1319,6 +1334,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1334,6 +1350,18 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1403,7 +1431,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1520,6 +1548,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1599,11 +1635,11 @@
   </sheetPr>
   <dimension ref="A1:AA988"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A170" activeCellId="0" sqref="A170"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A256" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B271" activeCellId="0" sqref="B271"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.43"/>
@@ -12131,7 +12167,7 @@
       <c r="Z250" s="7"/>
       <c r="AA250" s="7"/>
     </row>
-    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="8" t="s">
         <v>362</v>
       </c>
@@ -12629,7 +12665,7 @@
       <c r="C263" s="7"/>
       <c r="D263" s="7"/>
       <c r="E263" s="7" t="s">
-        <v>383</v>
+        <v>15</v>
       </c>
       <c r="F263" s="7"/>
       <c r="G263" s="26"/>
@@ -12659,12 +12695,12 @@
         <v>380</v>
       </c>
       <c r="B264" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C264" s="7"/>
       <c r="D264" s="7"/>
       <c r="E264" s="7" t="s">
-        <v>383</v>
+        <v>15</v>
       </c>
       <c r="F264" s="7"/>
       <c r="G264" s="26"/>
@@ -12691,7 +12727,7 @@
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B265" s="13" t="s">
         <v>381</v>
@@ -12732,7 +12768,7 @@
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B266" s="25" t="s">
         <v>382</v>
@@ -12767,10 +12803,10 @@
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B267" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C267" s="11"/>
       <c r="D267" s="11"/>
@@ -12800,15 +12836,29 @@
       <c r="Z267" s="7"/>
       <c r="AA267" s="7"/>
     </row>
-    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="7"/>
-      <c r="B268" s="7"/>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B268" s="28" t="s">
+        <v>386</v>
+      </c>
       <c r="C268" s="7"/>
-      <c r="D268" s="7"/>
-      <c r="E268" s="7"/>
+      <c r="D268" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="E268" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="F268" s="7"/>
-      <c r="G268" s="7"/>
-      <c r="H268" s="7"/>
+      <c r="G268" s="29" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H268" s="29" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
       <c r="I268" s="7"/>
       <c r="J268" s="7"/>
       <c r="K268" s="7"/>
@@ -12829,15 +12879,21 @@
       <c r="Z268" s="7"/>
       <c r="AA268" s="7"/>
     </row>
-    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="7"/>
-      <c r="B269" s="7"/>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B269" s="28" t="s">
+        <v>388</v>
+      </c>
       <c r="C269" s="7"/>
       <c r="D269" s="7"/>
-      <c r="E269" s="7"/>
+      <c r="E269" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F269" s="7"/>
-      <c r="G269" s="7"/>
-      <c r="H269" s="7"/>
+      <c r="G269" s="29"/>
+      <c r="H269" s="29"/>
       <c r="I269" s="7"/>
       <c r="J269" s="7"/>
       <c r="K269" s="7"/>
@@ -12858,15 +12914,21 @@
       <c r="Z269" s="7"/>
       <c r="AA269" s="7"/>
     </row>
-    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="7"/>
-      <c r="B270" s="7"/>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B270" s="28" t="s">
+        <v>389</v>
+      </c>
       <c r="C270" s="7"/>
       <c r="D270" s="7"/>
-      <c r="E270" s="7"/>
+      <c r="E270" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F270" s="7"/>
-      <c r="G270" s="7"/>
-      <c r="H270" s="7"/>
+      <c r="G270" s="29"/>
+      <c r="H270" s="29"/>
       <c r="I270" s="7"/>
       <c r="J270" s="7"/>
       <c r="K270" s="7"/>
@@ -12887,614 +12949,620 @@
       <c r="Z270" s="7"/>
       <c r="AA270" s="7"/>
     </row>
-    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="28"/>
-      <c r="B271" s="28"/>
-      <c r="C271" s="28"/>
-      <c r="D271" s="28"/>
-      <c r="E271" s="28"/>
-      <c r="F271" s="28"/>
-      <c r="G271" s="28"/>
-      <c r="H271" s="28"/>
-      <c r="I271" s="28"/>
-      <c r="J271" s="28"/>
-      <c r="K271" s="28"/>
-      <c r="L271" s="28"/>
-      <c r="M271" s="28"/>
-      <c r="N271" s="28"/>
-      <c r="O271" s="28"/>
-      <c r="P271" s="28"/>
-      <c r="Q271" s="28"/>
-      <c r="R271" s="28"/>
-      <c r="S271" s="28"/>
-      <c r="T271" s="28"/>
-      <c r="U271" s="28"/>
-      <c r="V271" s="28"/>
-      <c r="W271" s="28"/>
-      <c r="X271" s="28"/>
-      <c r="Y271" s="28"/>
-      <c r="Z271" s="28"/>
-      <c r="AA271" s="28"/>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="B271" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="C271" s="30"/>
+      <c r="D271" s="30"/>
+      <c r="E271" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F271" s="30"/>
+      <c r="G271" s="29"/>
+      <c r="H271" s="29"/>
+      <c r="I271" s="30"/>
+      <c r="J271" s="30"/>
+      <c r="K271" s="30"/>
+      <c r="L271" s="30"/>
+      <c r="M271" s="30"/>
+      <c r="N271" s="30"/>
+      <c r="O271" s="30"/>
+      <c r="P271" s="30"/>
+      <c r="Q271" s="30"/>
+      <c r="R271" s="30"/>
+      <c r="S271" s="30"/>
+      <c r="T271" s="30"/>
+      <c r="U271" s="30"/>
+      <c r="V271" s="30"/>
+      <c r="W271" s="30"/>
+      <c r="X271" s="30"/>
+      <c r="Y271" s="30"/>
+      <c r="Z271" s="30"/>
+      <c r="AA271" s="30"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="28"/>
-      <c r="B272" s="28"/>
-      <c r="C272" s="28"/>
-      <c r="D272" s="28"/>
-      <c r="E272" s="28"/>
-      <c r="F272" s="28"/>
-      <c r="G272" s="28"/>
-      <c r="H272" s="28"/>
-      <c r="I272" s="28"/>
-      <c r="J272" s="28"/>
-      <c r="K272" s="28"/>
-      <c r="L272" s="28"/>
-      <c r="M272" s="28"/>
-      <c r="N272" s="28"/>
-      <c r="O272" s="28"/>
-      <c r="P272" s="28"/>
-      <c r="Q272" s="28"/>
-      <c r="R272" s="28"/>
-      <c r="S272" s="28"/>
-      <c r="T272" s="28"/>
-      <c r="U272" s="28"/>
-      <c r="V272" s="28"/>
-      <c r="W272" s="28"/>
-      <c r="X272" s="28"/>
-      <c r="Y272" s="28"/>
-      <c r="Z272" s="28"/>
-      <c r="AA272" s="28"/>
+      <c r="A272" s="30"/>
+      <c r="B272" s="30"/>
+      <c r="C272" s="30"/>
+      <c r="D272" s="30"/>
+      <c r="E272" s="30"/>
+      <c r="F272" s="30"/>
+      <c r="G272" s="30"/>
+      <c r="H272" s="30"/>
+      <c r="I272" s="30"/>
+      <c r="J272" s="30"/>
+      <c r="K272" s="30"/>
+      <c r="L272" s="30"/>
+      <c r="M272" s="30"/>
+      <c r="N272" s="30"/>
+      <c r="O272" s="30"/>
+      <c r="P272" s="30"/>
+      <c r="Q272" s="30"/>
+      <c r="R272" s="30"/>
+      <c r="S272" s="30"/>
+      <c r="T272" s="30"/>
+      <c r="U272" s="30"/>
+      <c r="V272" s="30"/>
+      <c r="W272" s="30"/>
+      <c r="X272" s="30"/>
+      <c r="Y272" s="30"/>
+      <c r="Z272" s="30"/>
+      <c r="AA272" s="30"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="28"/>
-      <c r="B273" s="28"/>
-      <c r="C273" s="28"/>
-      <c r="D273" s="28"/>
-      <c r="E273" s="28"/>
-      <c r="F273" s="28"/>
-      <c r="G273" s="28"/>
-      <c r="H273" s="28"/>
-      <c r="I273" s="28"/>
-      <c r="J273" s="28"/>
-      <c r="K273" s="28"/>
-      <c r="L273" s="28"/>
-      <c r="M273" s="28"/>
-      <c r="N273" s="28"/>
-      <c r="O273" s="28"/>
-      <c r="P273" s="28"/>
-      <c r="Q273" s="28"/>
-      <c r="R273" s="28"/>
-      <c r="S273" s="28"/>
-      <c r="T273" s="28"/>
-      <c r="U273" s="28"/>
-      <c r="V273" s="28"/>
-      <c r="W273" s="28"/>
-      <c r="X273" s="28"/>
-      <c r="Y273" s="28"/>
-      <c r="Z273" s="28"/>
-      <c r="AA273" s="28"/>
+      <c r="A273" s="30"/>
+      <c r="B273" s="30"/>
+      <c r="C273" s="30"/>
+      <c r="D273" s="30"/>
+      <c r="E273" s="30"/>
+      <c r="F273" s="30"/>
+      <c r="G273" s="30"/>
+      <c r="H273" s="30"/>
+      <c r="I273" s="30"/>
+      <c r="J273" s="30"/>
+      <c r="K273" s="30"/>
+      <c r="L273" s="30"/>
+      <c r="M273" s="30"/>
+      <c r="N273" s="30"/>
+      <c r="O273" s="30"/>
+      <c r="P273" s="30"/>
+      <c r="Q273" s="30"/>
+      <c r="R273" s="30"/>
+      <c r="S273" s="30"/>
+      <c r="T273" s="30"/>
+      <c r="U273" s="30"/>
+      <c r="V273" s="30"/>
+      <c r="W273" s="30"/>
+      <c r="X273" s="30"/>
+      <c r="Y273" s="30"/>
+      <c r="Z273" s="30"/>
+      <c r="AA273" s="30"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="28"/>
-      <c r="B274" s="28"/>
-      <c r="C274" s="28"/>
-      <c r="D274" s="28"/>
-      <c r="E274" s="28"/>
-      <c r="F274" s="28"/>
-      <c r="G274" s="28"/>
-      <c r="H274" s="28"/>
-      <c r="I274" s="28"/>
-      <c r="J274" s="28"/>
-      <c r="K274" s="28"/>
-      <c r="L274" s="28"/>
-      <c r="M274" s="28"/>
-      <c r="N274" s="28"/>
-      <c r="O274" s="28"/>
-      <c r="P274" s="28"/>
-      <c r="Q274" s="28"/>
-      <c r="R274" s="28"/>
-      <c r="S274" s="28"/>
-      <c r="T274" s="28"/>
-      <c r="U274" s="28"/>
-      <c r="V274" s="28"/>
-      <c r="W274" s="28"/>
-      <c r="X274" s="28"/>
-      <c r="Y274" s="28"/>
-      <c r="Z274" s="28"/>
-      <c r="AA274" s="28"/>
+      <c r="A274" s="30"/>
+      <c r="B274" s="30"/>
+      <c r="C274" s="30"/>
+      <c r="D274" s="30"/>
+      <c r="E274" s="30"/>
+      <c r="F274" s="30"/>
+      <c r="G274" s="30"/>
+      <c r="H274" s="30"/>
+      <c r="I274" s="30"/>
+      <c r="J274" s="30"/>
+      <c r="K274" s="30"/>
+      <c r="L274" s="30"/>
+      <c r="M274" s="30"/>
+      <c r="N274" s="30"/>
+      <c r="O274" s="30"/>
+      <c r="P274" s="30"/>
+      <c r="Q274" s="30"/>
+      <c r="R274" s="30"/>
+      <c r="S274" s="30"/>
+      <c r="T274" s="30"/>
+      <c r="U274" s="30"/>
+      <c r="V274" s="30"/>
+      <c r="W274" s="30"/>
+      <c r="X274" s="30"/>
+      <c r="Y274" s="30"/>
+      <c r="Z274" s="30"/>
+      <c r="AA274" s="30"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="28"/>
-      <c r="B275" s="28"/>
-      <c r="C275" s="28"/>
-      <c r="D275" s="28"/>
-      <c r="E275" s="28"/>
-      <c r="F275" s="28"/>
-      <c r="G275" s="28"/>
-      <c r="H275" s="28"/>
-      <c r="I275" s="28"/>
-      <c r="J275" s="28"/>
-      <c r="K275" s="28"/>
-      <c r="L275" s="28"/>
-      <c r="M275" s="28"/>
-      <c r="N275" s="28"/>
-      <c r="O275" s="28"/>
-      <c r="P275" s="28"/>
-      <c r="Q275" s="28"/>
-      <c r="R275" s="28"/>
-      <c r="S275" s="28"/>
-      <c r="T275" s="28"/>
-      <c r="U275" s="28"/>
-      <c r="V275" s="28"/>
-      <c r="W275" s="28"/>
-      <c r="X275" s="28"/>
-      <c r="Y275" s="28"/>
-      <c r="Z275" s="28"/>
-      <c r="AA275" s="28"/>
+      <c r="A275" s="30"/>
+      <c r="B275" s="30"/>
+      <c r="C275" s="30"/>
+      <c r="D275" s="30"/>
+      <c r="E275" s="30"/>
+      <c r="F275" s="30"/>
+      <c r="G275" s="30"/>
+      <c r="H275" s="30"/>
+      <c r="I275" s="30"/>
+      <c r="J275" s="30"/>
+      <c r="K275" s="30"/>
+      <c r="L275" s="30"/>
+      <c r="M275" s="30"/>
+      <c r="N275" s="30"/>
+      <c r="O275" s="30"/>
+      <c r="P275" s="30"/>
+      <c r="Q275" s="30"/>
+      <c r="R275" s="30"/>
+      <c r="S275" s="30"/>
+      <c r="T275" s="30"/>
+      <c r="U275" s="30"/>
+      <c r="V275" s="30"/>
+      <c r="W275" s="30"/>
+      <c r="X275" s="30"/>
+      <c r="Y275" s="30"/>
+      <c r="Z275" s="30"/>
+      <c r="AA275" s="30"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="28"/>
-      <c r="B276" s="28"/>
-      <c r="C276" s="28"/>
-      <c r="D276" s="28"/>
-      <c r="E276" s="28"/>
-      <c r="F276" s="28"/>
-      <c r="G276" s="28"/>
-      <c r="H276" s="28"/>
-      <c r="I276" s="28"/>
-      <c r="J276" s="28"/>
-      <c r="K276" s="28"/>
-      <c r="L276" s="28"/>
-      <c r="M276" s="28"/>
-      <c r="N276" s="28"/>
-      <c r="O276" s="28"/>
-      <c r="P276" s="28"/>
-      <c r="Q276" s="28"/>
-      <c r="R276" s="28"/>
-      <c r="S276" s="28"/>
-      <c r="T276" s="28"/>
-      <c r="U276" s="28"/>
-      <c r="V276" s="28"/>
-      <c r="W276" s="28"/>
-      <c r="X276" s="28"/>
-      <c r="Y276" s="28"/>
-      <c r="Z276" s="28"/>
-      <c r="AA276" s="28"/>
+      <c r="A276" s="30"/>
+      <c r="B276" s="30"/>
+      <c r="C276" s="30"/>
+      <c r="D276" s="30"/>
+      <c r="E276" s="30"/>
+      <c r="F276" s="30"/>
+      <c r="G276" s="30"/>
+      <c r="H276" s="30"/>
+      <c r="I276" s="30"/>
+      <c r="J276" s="30"/>
+      <c r="K276" s="30"/>
+      <c r="L276" s="30"/>
+      <c r="M276" s="30"/>
+      <c r="N276" s="30"/>
+      <c r="O276" s="30"/>
+      <c r="P276" s="30"/>
+      <c r="Q276" s="30"/>
+      <c r="R276" s="30"/>
+      <c r="S276" s="30"/>
+      <c r="T276" s="30"/>
+      <c r="U276" s="30"/>
+      <c r="V276" s="30"/>
+      <c r="W276" s="30"/>
+      <c r="X276" s="30"/>
+      <c r="Y276" s="30"/>
+      <c r="Z276" s="30"/>
+      <c r="AA276" s="30"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="28"/>
-      <c r="B277" s="28"/>
-      <c r="C277" s="28"/>
-      <c r="D277" s="28"/>
-      <c r="E277" s="28"/>
-      <c r="F277" s="28"/>
-      <c r="G277" s="28"/>
-      <c r="H277" s="28"/>
-      <c r="I277" s="28"/>
-      <c r="J277" s="28"/>
-      <c r="K277" s="28"/>
-      <c r="L277" s="28"/>
-      <c r="M277" s="28"/>
-      <c r="N277" s="28"/>
-      <c r="O277" s="28"/>
-      <c r="P277" s="28"/>
-      <c r="Q277" s="28"/>
-      <c r="R277" s="28"/>
-      <c r="S277" s="28"/>
-      <c r="T277" s="28"/>
-      <c r="U277" s="28"/>
-      <c r="V277" s="28"/>
-      <c r="W277" s="28"/>
-      <c r="X277" s="28"/>
-      <c r="Y277" s="28"/>
-      <c r="Z277" s="28"/>
-      <c r="AA277" s="28"/>
+      <c r="A277" s="30"/>
+      <c r="B277" s="30"/>
+      <c r="C277" s="30"/>
+      <c r="D277" s="30"/>
+      <c r="E277" s="30"/>
+      <c r="F277" s="30"/>
+      <c r="G277" s="30"/>
+      <c r="H277" s="30"/>
+      <c r="I277" s="30"/>
+      <c r="J277" s="30"/>
+      <c r="K277" s="30"/>
+      <c r="L277" s="30"/>
+      <c r="M277" s="30"/>
+      <c r="N277" s="30"/>
+      <c r="O277" s="30"/>
+      <c r="P277" s="30"/>
+      <c r="Q277" s="30"/>
+      <c r="R277" s="30"/>
+      <c r="S277" s="30"/>
+      <c r="T277" s="30"/>
+      <c r="U277" s="30"/>
+      <c r="V277" s="30"/>
+      <c r="W277" s="30"/>
+      <c r="X277" s="30"/>
+      <c r="Y277" s="30"/>
+      <c r="Z277" s="30"/>
+      <c r="AA277" s="30"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="28"/>
-      <c r="B278" s="28"/>
-      <c r="C278" s="28"/>
-      <c r="D278" s="28"/>
-      <c r="E278" s="28"/>
-      <c r="F278" s="28"/>
-      <c r="G278" s="28"/>
-      <c r="H278" s="28"/>
-      <c r="I278" s="28"/>
-      <c r="J278" s="28"/>
-      <c r="K278" s="28"/>
-      <c r="L278" s="28"/>
-      <c r="M278" s="28"/>
-      <c r="N278" s="28"/>
-      <c r="O278" s="28"/>
-      <c r="P278" s="28"/>
-      <c r="Q278" s="28"/>
-      <c r="R278" s="28"/>
-      <c r="S278" s="28"/>
-      <c r="T278" s="28"/>
-      <c r="U278" s="28"/>
-      <c r="V278" s="28"/>
-      <c r="W278" s="28"/>
-      <c r="X278" s="28"/>
-      <c r="Y278" s="28"/>
-      <c r="Z278" s="28"/>
-      <c r="AA278" s="28"/>
+      <c r="A278" s="30"/>
+      <c r="B278" s="30"/>
+      <c r="C278" s="30"/>
+      <c r="D278" s="30"/>
+      <c r="E278" s="30"/>
+      <c r="F278" s="30"/>
+      <c r="G278" s="30"/>
+      <c r="H278" s="30"/>
+      <c r="I278" s="30"/>
+      <c r="J278" s="30"/>
+      <c r="K278" s="30"/>
+      <c r="L278" s="30"/>
+      <c r="M278" s="30"/>
+      <c r="N278" s="30"/>
+      <c r="O278" s="30"/>
+      <c r="P278" s="30"/>
+      <c r="Q278" s="30"/>
+      <c r="R278" s="30"/>
+      <c r="S278" s="30"/>
+      <c r="T278" s="30"/>
+      <c r="U278" s="30"/>
+      <c r="V278" s="30"/>
+      <c r="W278" s="30"/>
+      <c r="X278" s="30"/>
+      <c r="Y278" s="30"/>
+      <c r="Z278" s="30"/>
+      <c r="AA278" s="30"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="28"/>
-      <c r="B279" s="28"/>
-      <c r="C279" s="28"/>
-      <c r="D279" s="28"/>
-      <c r="E279" s="28"/>
-      <c r="F279" s="28"/>
-      <c r="G279" s="28"/>
-      <c r="H279" s="28"/>
-      <c r="I279" s="28"/>
-      <c r="J279" s="28"/>
-      <c r="K279" s="28"/>
-      <c r="L279" s="28"/>
-      <c r="M279" s="28"/>
-      <c r="N279" s="28"/>
-      <c r="O279" s="28"/>
-      <c r="P279" s="28"/>
-      <c r="Q279" s="28"/>
-      <c r="R279" s="28"/>
-      <c r="S279" s="28"/>
-      <c r="T279" s="28"/>
-      <c r="U279" s="28"/>
-      <c r="V279" s="28"/>
-      <c r="W279" s="28"/>
-      <c r="X279" s="28"/>
-      <c r="Y279" s="28"/>
-      <c r="Z279" s="28"/>
-      <c r="AA279" s="28"/>
+      <c r="A279" s="30"/>
+      <c r="B279" s="30"/>
+      <c r="C279" s="30"/>
+      <c r="D279" s="30"/>
+      <c r="E279" s="30"/>
+      <c r="F279" s="30"/>
+      <c r="G279" s="30"/>
+      <c r="H279" s="30"/>
+      <c r="I279" s="30"/>
+      <c r="J279" s="30"/>
+      <c r="K279" s="30"/>
+      <c r="L279" s="30"/>
+      <c r="M279" s="30"/>
+      <c r="N279" s="30"/>
+      <c r="O279" s="30"/>
+      <c r="P279" s="30"/>
+      <c r="Q279" s="30"/>
+      <c r="R279" s="30"/>
+      <c r="S279" s="30"/>
+      <c r="T279" s="30"/>
+      <c r="U279" s="30"/>
+      <c r="V279" s="30"/>
+      <c r="W279" s="30"/>
+      <c r="X279" s="30"/>
+      <c r="Y279" s="30"/>
+      <c r="Z279" s="30"/>
+      <c r="AA279" s="30"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="28"/>
-      <c r="B280" s="28"/>
-      <c r="C280" s="28"/>
-      <c r="D280" s="28"/>
-      <c r="E280" s="28"/>
-      <c r="F280" s="28"/>
-      <c r="G280" s="28"/>
-      <c r="H280" s="28"/>
-      <c r="I280" s="28"/>
-      <c r="J280" s="28"/>
-      <c r="K280" s="28"/>
-      <c r="L280" s="28"/>
-      <c r="M280" s="28"/>
-      <c r="N280" s="28"/>
-      <c r="O280" s="28"/>
-      <c r="P280" s="28"/>
-      <c r="Q280" s="28"/>
-      <c r="R280" s="28"/>
-      <c r="S280" s="28"/>
-      <c r="T280" s="28"/>
-      <c r="U280" s="28"/>
-      <c r="V280" s="28"/>
-      <c r="W280" s="28"/>
-      <c r="X280" s="28"/>
-      <c r="Y280" s="28"/>
-      <c r="Z280" s="28"/>
-      <c r="AA280" s="28"/>
+      <c r="A280" s="30"/>
+      <c r="B280" s="30"/>
+      <c r="C280" s="30"/>
+      <c r="D280" s="30"/>
+      <c r="E280" s="30"/>
+      <c r="F280" s="30"/>
+      <c r="G280" s="30"/>
+      <c r="H280" s="30"/>
+      <c r="I280" s="30"/>
+      <c r="J280" s="30"/>
+      <c r="K280" s="30"/>
+      <c r="L280" s="30"/>
+      <c r="M280" s="30"/>
+      <c r="N280" s="30"/>
+      <c r="O280" s="30"/>
+      <c r="P280" s="30"/>
+      <c r="Q280" s="30"/>
+      <c r="R280" s="30"/>
+      <c r="S280" s="30"/>
+      <c r="T280" s="30"/>
+      <c r="U280" s="30"/>
+      <c r="V280" s="30"/>
+      <c r="W280" s="30"/>
+      <c r="X280" s="30"/>
+      <c r="Y280" s="30"/>
+      <c r="Z280" s="30"/>
+      <c r="AA280" s="30"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="28"/>
-      <c r="B281" s="28"/>
-      <c r="C281" s="28"/>
-      <c r="D281" s="28"/>
-      <c r="E281" s="28"/>
-      <c r="F281" s="28"/>
-      <c r="G281" s="28"/>
-      <c r="H281" s="28"/>
-      <c r="I281" s="28"/>
-      <c r="J281" s="28"/>
-      <c r="K281" s="28"/>
-      <c r="L281" s="28"/>
-      <c r="M281" s="28"/>
-      <c r="N281" s="28"/>
-      <c r="O281" s="28"/>
-      <c r="P281" s="28"/>
-      <c r="Q281" s="28"/>
-      <c r="R281" s="28"/>
-      <c r="S281" s="28"/>
-      <c r="T281" s="28"/>
-      <c r="U281" s="28"/>
-      <c r="V281" s="28"/>
-      <c r="W281" s="28"/>
-      <c r="X281" s="28"/>
-      <c r="Y281" s="28"/>
-      <c r="Z281" s="28"/>
-      <c r="AA281" s="28"/>
+      <c r="A281" s="30"/>
+      <c r="B281" s="30"/>
+      <c r="C281" s="30"/>
+      <c r="D281" s="30"/>
+      <c r="E281" s="30"/>
+      <c r="F281" s="30"/>
+      <c r="G281" s="30"/>
+      <c r="H281" s="30"/>
+      <c r="I281" s="30"/>
+      <c r="J281" s="30"/>
+      <c r="K281" s="30"/>
+      <c r="L281" s="30"/>
+      <c r="M281" s="30"/>
+      <c r="N281" s="30"/>
+      <c r="O281" s="30"/>
+      <c r="P281" s="30"/>
+      <c r="Q281" s="30"/>
+      <c r="R281" s="30"/>
+      <c r="S281" s="30"/>
+      <c r="T281" s="30"/>
+      <c r="U281" s="30"/>
+      <c r="V281" s="30"/>
+      <c r="W281" s="30"/>
+      <c r="X281" s="30"/>
+      <c r="Y281" s="30"/>
+      <c r="Z281" s="30"/>
+      <c r="AA281" s="30"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="28"/>
-      <c r="B282" s="28"/>
-      <c r="C282" s="28"/>
-      <c r="D282" s="28"/>
-      <c r="E282" s="28"/>
-      <c r="F282" s="28"/>
-      <c r="G282" s="28"/>
-      <c r="H282" s="28"/>
-      <c r="I282" s="28"/>
-      <c r="J282" s="28"/>
-      <c r="K282" s="28"/>
-      <c r="L282" s="28"/>
-      <c r="M282" s="28"/>
-      <c r="N282" s="28"/>
-      <c r="O282" s="28"/>
-      <c r="P282" s="28"/>
-      <c r="Q282" s="28"/>
-      <c r="R282" s="28"/>
-      <c r="S282" s="28"/>
-      <c r="T282" s="28"/>
-      <c r="U282" s="28"/>
-      <c r="V282" s="28"/>
-      <c r="W282" s="28"/>
-      <c r="X282" s="28"/>
-      <c r="Y282" s="28"/>
-      <c r="Z282" s="28"/>
-      <c r="AA282" s="28"/>
+      <c r="A282" s="30"/>
+      <c r="B282" s="30"/>
+      <c r="C282" s="30"/>
+      <c r="D282" s="30"/>
+      <c r="E282" s="30"/>
+      <c r="F282" s="30"/>
+      <c r="G282" s="30"/>
+      <c r="H282" s="30"/>
+      <c r="I282" s="30"/>
+      <c r="J282" s="30"/>
+      <c r="K282" s="30"/>
+      <c r="L282" s="30"/>
+      <c r="M282" s="30"/>
+      <c r="N282" s="30"/>
+      <c r="O282" s="30"/>
+      <c r="P282" s="30"/>
+      <c r="Q282" s="30"/>
+      <c r="R282" s="30"/>
+      <c r="S282" s="30"/>
+      <c r="T282" s="30"/>
+      <c r="U282" s="30"/>
+      <c r="V282" s="30"/>
+      <c r="W282" s="30"/>
+      <c r="X282" s="30"/>
+      <c r="Y282" s="30"/>
+      <c r="Z282" s="30"/>
+      <c r="AA282" s="30"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="28"/>
-      <c r="B283" s="28"/>
-      <c r="C283" s="28"/>
-      <c r="D283" s="28"/>
-      <c r="E283" s="28"/>
-      <c r="F283" s="28"/>
-      <c r="G283" s="28"/>
-      <c r="H283" s="28"/>
-      <c r="I283" s="28"/>
-      <c r="J283" s="28"/>
-      <c r="K283" s="28"/>
-      <c r="L283" s="28"/>
-      <c r="M283" s="28"/>
-      <c r="N283" s="28"/>
-      <c r="O283" s="28"/>
-      <c r="P283" s="28"/>
-      <c r="Q283" s="28"/>
-      <c r="R283" s="28"/>
-      <c r="S283" s="28"/>
-      <c r="T283" s="28"/>
-      <c r="U283" s="28"/>
-      <c r="V283" s="28"/>
-      <c r="W283" s="28"/>
-      <c r="X283" s="28"/>
-      <c r="Y283" s="28"/>
-      <c r="Z283" s="28"/>
-      <c r="AA283" s="28"/>
+      <c r="A283" s="30"/>
+      <c r="B283" s="30"/>
+      <c r="C283" s="30"/>
+      <c r="D283" s="30"/>
+      <c r="E283" s="30"/>
+      <c r="F283" s="30"/>
+      <c r="G283" s="30"/>
+      <c r="H283" s="30"/>
+      <c r="I283" s="30"/>
+      <c r="J283" s="30"/>
+      <c r="K283" s="30"/>
+      <c r="L283" s="30"/>
+      <c r="M283" s="30"/>
+      <c r="N283" s="30"/>
+      <c r="O283" s="30"/>
+      <c r="P283" s="30"/>
+      <c r="Q283" s="30"/>
+      <c r="R283" s="30"/>
+      <c r="S283" s="30"/>
+      <c r="T283" s="30"/>
+      <c r="U283" s="30"/>
+      <c r="V283" s="30"/>
+      <c r="W283" s="30"/>
+      <c r="X283" s="30"/>
+      <c r="Y283" s="30"/>
+      <c r="Z283" s="30"/>
+      <c r="AA283" s="30"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="28"/>
-      <c r="B284" s="28"/>
-      <c r="C284" s="28"/>
-      <c r="D284" s="28"/>
-      <c r="E284" s="28"/>
-      <c r="F284" s="28"/>
-      <c r="G284" s="28"/>
-      <c r="H284" s="28"/>
-      <c r="I284" s="28"/>
-      <c r="J284" s="28"/>
-      <c r="K284" s="28"/>
-      <c r="L284" s="28"/>
-      <c r="M284" s="28"/>
-      <c r="N284" s="28"/>
-      <c r="O284" s="28"/>
-      <c r="P284" s="28"/>
-      <c r="Q284" s="28"/>
-      <c r="R284" s="28"/>
-      <c r="S284" s="28"/>
-      <c r="T284" s="28"/>
-      <c r="U284" s="28"/>
-      <c r="V284" s="28"/>
-      <c r="W284" s="28"/>
-      <c r="X284" s="28"/>
-      <c r="Y284" s="28"/>
-      <c r="Z284" s="28"/>
-      <c r="AA284" s="28"/>
+      <c r="A284" s="30"/>
+      <c r="B284" s="30"/>
+      <c r="C284" s="30"/>
+      <c r="D284" s="30"/>
+      <c r="E284" s="30"/>
+      <c r="F284" s="30"/>
+      <c r="G284" s="30"/>
+      <c r="H284" s="30"/>
+      <c r="I284" s="30"/>
+      <c r="J284" s="30"/>
+      <c r="K284" s="30"/>
+      <c r="L284" s="30"/>
+      <c r="M284" s="30"/>
+      <c r="N284" s="30"/>
+      <c r="O284" s="30"/>
+      <c r="P284" s="30"/>
+      <c r="Q284" s="30"/>
+      <c r="R284" s="30"/>
+      <c r="S284" s="30"/>
+      <c r="T284" s="30"/>
+      <c r="U284" s="30"/>
+      <c r="V284" s="30"/>
+      <c r="W284" s="30"/>
+      <c r="X284" s="30"/>
+      <c r="Y284" s="30"/>
+      <c r="Z284" s="30"/>
+      <c r="AA284" s="30"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="28"/>
-      <c r="B285" s="28"/>
-      <c r="C285" s="28"/>
-      <c r="D285" s="28"/>
-      <c r="E285" s="28"/>
-      <c r="F285" s="28"/>
-      <c r="G285" s="28"/>
-      <c r="H285" s="28"/>
-      <c r="I285" s="28"/>
-      <c r="J285" s="28"/>
-      <c r="K285" s="28"/>
-      <c r="L285" s="28"/>
-      <c r="M285" s="28"/>
-      <c r="N285" s="28"/>
-      <c r="O285" s="28"/>
-      <c r="P285" s="28"/>
-      <c r="Q285" s="28"/>
-      <c r="R285" s="28"/>
-      <c r="S285" s="28"/>
-      <c r="T285" s="28"/>
-      <c r="U285" s="28"/>
-      <c r="V285" s="28"/>
-      <c r="W285" s="28"/>
-      <c r="X285" s="28"/>
-      <c r="Y285" s="28"/>
-      <c r="Z285" s="28"/>
-      <c r="AA285" s="28"/>
+      <c r="A285" s="30"/>
+      <c r="B285" s="30"/>
+      <c r="C285" s="30"/>
+      <c r="D285" s="30"/>
+      <c r="E285" s="30"/>
+      <c r="F285" s="30"/>
+      <c r="G285" s="30"/>
+      <c r="H285" s="30"/>
+      <c r="I285" s="30"/>
+      <c r="J285" s="30"/>
+      <c r="K285" s="30"/>
+      <c r="L285" s="30"/>
+      <c r="M285" s="30"/>
+      <c r="N285" s="30"/>
+      <c r="O285" s="30"/>
+      <c r="P285" s="30"/>
+      <c r="Q285" s="30"/>
+      <c r="R285" s="30"/>
+      <c r="S285" s="30"/>
+      <c r="T285" s="30"/>
+      <c r="U285" s="30"/>
+      <c r="V285" s="30"/>
+      <c r="W285" s="30"/>
+      <c r="X285" s="30"/>
+      <c r="Y285" s="30"/>
+      <c r="Z285" s="30"/>
+      <c r="AA285" s="30"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="28"/>
-      <c r="B286" s="28"/>
-      <c r="C286" s="28"/>
-      <c r="D286" s="28"/>
-      <c r="E286" s="28"/>
-      <c r="F286" s="28"/>
-      <c r="G286" s="28"/>
-      <c r="H286" s="28"/>
-      <c r="I286" s="28"/>
-      <c r="J286" s="28"/>
-      <c r="K286" s="28"/>
-      <c r="L286" s="28"/>
-      <c r="M286" s="28"/>
-      <c r="N286" s="28"/>
-      <c r="O286" s="28"/>
-      <c r="P286" s="28"/>
-      <c r="Q286" s="28"/>
-      <c r="R286" s="28"/>
-      <c r="S286" s="28"/>
-      <c r="T286" s="28"/>
-      <c r="U286" s="28"/>
-      <c r="V286" s="28"/>
-      <c r="W286" s="28"/>
-      <c r="X286" s="28"/>
-      <c r="Y286" s="28"/>
-      <c r="Z286" s="28"/>
-      <c r="AA286" s="28"/>
+      <c r="A286" s="30"/>
+      <c r="B286" s="30"/>
+      <c r="C286" s="30"/>
+      <c r="D286" s="30"/>
+      <c r="E286" s="30"/>
+      <c r="F286" s="30"/>
+      <c r="G286" s="30"/>
+      <c r="H286" s="30"/>
+      <c r="I286" s="30"/>
+      <c r="J286" s="30"/>
+      <c r="K286" s="30"/>
+      <c r="L286" s="30"/>
+      <c r="M286" s="30"/>
+      <c r="N286" s="30"/>
+      <c r="O286" s="30"/>
+      <c r="P286" s="30"/>
+      <c r="Q286" s="30"/>
+      <c r="R286" s="30"/>
+      <c r="S286" s="30"/>
+      <c r="T286" s="30"/>
+      <c r="U286" s="30"/>
+      <c r="V286" s="30"/>
+      <c r="W286" s="30"/>
+      <c r="X286" s="30"/>
+      <c r="Y286" s="30"/>
+      <c r="Z286" s="30"/>
+      <c r="AA286" s="30"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="28"/>
-      <c r="B287" s="28"/>
-      <c r="C287" s="28"/>
-      <c r="D287" s="28"/>
-      <c r="E287" s="28"/>
-      <c r="F287" s="28"/>
-      <c r="G287" s="28"/>
-      <c r="H287" s="28"/>
-      <c r="I287" s="28"/>
-      <c r="J287" s="28"/>
-      <c r="K287" s="28"/>
-      <c r="L287" s="28"/>
-      <c r="M287" s="28"/>
-      <c r="N287" s="28"/>
-      <c r="O287" s="28"/>
-      <c r="P287" s="28"/>
-      <c r="Q287" s="28"/>
-      <c r="R287" s="28"/>
-      <c r="S287" s="28"/>
-      <c r="T287" s="28"/>
-      <c r="U287" s="28"/>
-      <c r="V287" s="28"/>
-      <c r="W287" s="28"/>
-      <c r="X287" s="28"/>
-      <c r="Y287" s="28"/>
-      <c r="Z287" s="28"/>
-      <c r="AA287" s="28"/>
+      <c r="A287" s="30"/>
+      <c r="B287" s="30"/>
+      <c r="C287" s="30"/>
+      <c r="D287" s="30"/>
+      <c r="E287" s="30"/>
+      <c r="F287" s="30"/>
+      <c r="G287" s="30"/>
+      <c r="H287" s="30"/>
+      <c r="I287" s="30"/>
+      <c r="J287" s="30"/>
+      <c r="K287" s="30"/>
+      <c r="L287" s="30"/>
+      <c r="M287" s="30"/>
+      <c r="N287" s="30"/>
+      <c r="O287" s="30"/>
+      <c r="P287" s="30"/>
+      <c r="Q287" s="30"/>
+      <c r="R287" s="30"/>
+      <c r="S287" s="30"/>
+      <c r="T287" s="30"/>
+      <c r="U287" s="30"/>
+      <c r="V287" s="30"/>
+      <c r="W287" s="30"/>
+      <c r="X287" s="30"/>
+      <c r="Y287" s="30"/>
+      <c r="Z287" s="30"/>
+      <c r="AA287" s="30"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="28"/>
-      <c r="B288" s="28"/>
-      <c r="C288" s="28"/>
-      <c r="D288" s="28"/>
-      <c r="E288" s="28"/>
-      <c r="F288" s="28"/>
-      <c r="G288" s="28"/>
-      <c r="H288" s="28"/>
-      <c r="I288" s="28"/>
-      <c r="J288" s="28"/>
-      <c r="K288" s="28"/>
-      <c r="L288" s="28"/>
-      <c r="M288" s="28"/>
-      <c r="N288" s="28"/>
-      <c r="O288" s="28"/>
-      <c r="P288" s="28"/>
-      <c r="Q288" s="28"/>
-      <c r="R288" s="28"/>
-      <c r="S288" s="28"/>
-      <c r="T288" s="28"/>
-      <c r="U288" s="28"/>
-      <c r="V288" s="28"/>
-      <c r="W288" s="28"/>
-      <c r="X288" s="28"/>
-      <c r="Y288" s="28"/>
-      <c r="Z288" s="28"/>
-      <c r="AA288" s="28"/>
+      <c r="A288" s="30"/>
+      <c r="B288" s="30"/>
+      <c r="C288" s="30"/>
+      <c r="D288" s="30"/>
+      <c r="E288" s="30"/>
+      <c r="F288" s="30"/>
+      <c r="G288" s="30"/>
+      <c r="H288" s="30"/>
+      <c r="I288" s="30"/>
+      <c r="J288" s="30"/>
+      <c r="K288" s="30"/>
+      <c r="L288" s="30"/>
+      <c r="M288" s="30"/>
+      <c r="N288" s="30"/>
+      <c r="O288" s="30"/>
+      <c r="P288" s="30"/>
+      <c r="Q288" s="30"/>
+      <c r="R288" s="30"/>
+      <c r="S288" s="30"/>
+      <c r="T288" s="30"/>
+      <c r="U288" s="30"/>
+      <c r="V288" s="30"/>
+      <c r="W288" s="30"/>
+      <c r="X288" s="30"/>
+      <c r="Y288" s="30"/>
+      <c r="Z288" s="30"/>
+      <c r="AA288" s="30"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="28"/>
-      <c r="B289" s="28"/>
-      <c r="C289" s="28"/>
-      <c r="D289" s="28"/>
-      <c r="E289" s="28"/>
-      <c r="F289" s="28"/>
-      <c r="G289" s="28"/>
-      <c r="H289" s="28"/>
-      <c r="I289" s="28"/>
-      <c r="J289" s="28"/>
-      <c r="K289" s="28"/>
-      <c r="L289" s="28"/>
-      <c r="M289" s="28"/>
-      <c r="N289" s="28"/>
-      <c r="O289" s="28"/>
-      <c r="P289" s="28"/>
-      <c r="Q289" s="28"/>
-      <c r="R289" s="28"/>
-      <c r="S289" s="28"/>
-      <c r="T289" s="28"/>
-      <c r="U289" s="28"/>
-      <c r="V289" s="28"/>
-      <c r="W289" s="28"/>
-      <c r="X289" s="28"/>
-      <c r="Y289" s="28"/>
-      <c r="Z289" s="28"/>
-      <c r="AA289" s="28"/>
+      <c r="A289" s="30"/>
+      <c r="B289" s="30"/>
+      <c r="C289" s="30"/>
+      <c r="D289" s="30"/>
+      <c r="E289" s="30"/>
+      <c r="F289" s="30"/>
+      <c r="G289" s="30"/>
+      <c r="H289" s="30"/>
+      <c r="I289" s="30"/>
+      <c r="J289" s="30"/>
+      <c r="K289" s="30"/>
+      <c r="L289" s="30"/>
+      <c r="M289" s="30"/>
+      <c r="N289" s="30"/>
+      <c r="O289" s="30"/>
+      <c r="P289" s="30"/>
+      <c r="Q289" s="30"/>
+      <c r="R289" s="30"/>
+      <c r="S289" s="30"/>
+      <c r="T289" s="30"/>
+      <c r="U289" s="30"/>
+      <c r="V289" s="30"/>
+      <c r="W289" s="30"/>
+      <c r="X289" s="30"/>
+      <c r="Y289" s="30"/>
+      <c r="Z289" s="30"/>
+      <c r="AA289" s="30"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="28"/>
-      <c r="B290" s="28"/>
-      <c r="C290" s="28"/>
-      <c r="D290" s="28"/>
-      <c r="E290" s="28"/>
-      <c r="F290" s="28"/>
-      <c r="G290" s="28"/>
-      <c r="H290" s="28"/>
-      <c r="I290" s="28"/>
-      <c r="J290" s="28"/>
-      <c r="K290" s="28"/>
-      <c r="L290" s="28"/>
-      <c r="M290" s="28"/>
-      <c r="N290" s="28"/>
-      <c r="O290" s="28"/>
-      <c r="P290" s="28"/>
-      <c r="Q290" s="28"/>
-      <c r="R290" s="28"/>
-      <c r="S290" s="28"/>
-      <c r="T290" s="28"/>
-      <c r="U290" s="28"/>
-      <c r="V290" s="28"/>
-      <c r="W290" s="28"/>
-      <c r="X290" s="28"/>
-      <c r="Y290" s="28"/>
-      <c r="Z290" s="28"/>
-      <c r="AA290" s="28"/>
+      <c r="A290" s="30"/>
+      <c r="B290" s="30"/>
+      <c r="C290" s="30"/>
+      <c r="D290" s="30"/>
+      <c r="E290" s="30"/>
+      <c r="F290" s="30"/>
+      <c r="G290" s="30"/>
+      <c r="H290" s="30"/>
+      <c r="I290" s="30"/>
+      <c r="J290" s="30"/>
+      <c r="K290" s="30"/>
+      <c r="L290" s="30"/>
+      <c r="M290" s="30"/>
+      <c r="N290" s="30"/>
+      <c r="O290" s="30"/>
+      <c r="P290" s="30"/>
+      <c r="Q290" s="30"/>
+      <c r="R290" s="30"/>
+      <c r="S290" s="30"/>
+      <c r="T290" s="30"/>
+      <c r="U290" s="30"/>
+      <c r="V290" s="30"/>
+      <c r="W290" s="30"/>
+      <c r="X290" s="30"/>
+      <c r="Y290" s="30"/>
+      <c r="Z290" s="30"/>
+      <c r="AA290" s="30"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="28"/>
-      <c r="B291" s="28"/>
-      <c r="C291" s="28"/>
-      <c r="D291" s="28"/>
-      <c r="E291" s="28"/>
-      <c r="F291" s="28"/>
-      <c r="G291" s="28"/>
-      <c r="H291" s="28"/>
-      <c r="I291" s="28"/>
-      <c r="J291" s="28"/>
-      <c r="K291" s="28"/>
-      <c r="L291" s="28"/>
-      <c r="M291" s="28"/>
-      <c r="N291" s="28"/>
-      <c r="O291" s="28"/>
-      <c r="P291" s="28"/>
-      <c r="Q291" s="28"/>
-      <c r="R291" s="28"/>
-      <c r="S291" s="28"/>
-      <c r="T291" s="28"/>
-      <c r="U291" s="28"/>
-      <c r="V291" s="28"/>
-      <c r="W291" s="28"/>
-      <c r="X291" s="28"/>
-      <c r="Y291" s="28"/>
-      <c r="Z291" s="28"/>
-      <c r="AA291" s="28"/>
+      <c r="A291" s="30"/>
+      <c r="B291" s="30"/>
+      <c r="C291" s="30"/>
+      <c r="D291" s="30"/>
+      <c r="E291" s="30"/>
+      <c r="F291" s="30"/>
+      <c r="G291" s="30"/>
+      <c r="H291" s="30"/>
+      <c r="I291" s="30"/>
+      <c r="J291" s="30"/>
+      <c r="K291" s="30"/>
+      <c r="L291" s="30"/>
+      <c r="M291" s="30"/>
+      <c r="N291" s="30"/>
+      <c r="O291" s="30"/>
+      <c r="P291" s="30"/>
+      <c r="Q291" s="30"/>
+      <c r="R291" s="30"/>
+      <c r="S291" s="30"/>
+      <c r="T291" s="30"/>
+      <c r="U291" s="30"/>
+      <c r="V291" s="30"/>
+      <c r="W291" s="30"/>
+      <c r="X291" s="30"/>
+      <c r="Y291" s="30"/>
+      <c r="Z291" s="30"/>
+      <c r="AA291" s="30"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="27"/>
@@ -19073,7 +19141,7 @@
       <c r="F988" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="156">
+  <mergeCells count="158">
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="G6:G9"/>
@@ -19230,9 +19298,11 @@
     <mergeCell ref="H262:H264"/>
     <mergeCell ref="G265:G267"/>
     <mergeCell ref="H265:H267"/>
+    <mergeCell ref="G268:G271"/>
+    <mergeCell ref="H268:H271"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D94" r:id="rId2" display="ckremen@berkeley.edu"/>
+    <hyperlink ref="D94" r:id="rId2" display="ckremen@berkeley.edu "/>
     <hyperlink ref="D167" r:id="rId3" display="hlc66@cornell.edu"/>
     <hyperlink ref="D168" r:id="rId4" display="hlc66@cornell.edu"/>
     <hyperlink ref="D169" r:id="rId5" display="hlc66@cornell.edu"/>
@@ -19241,6 +19311,7 @@
     <hyperlink ref="D189" r:id="rId8" display="smithakrishnan@gmail.com"/>
     <hyperlink ref="D221" r:id="rId9" display="davilramos91@gmail.com"/>
     <hyperlink ref="C241" r:id="rId10" display="https://snd.gu.se/en/catalogue/study/by-topic"/>
+    <hyperlink ref="D251" r:id="rId11" display="bwillcox@myune.edu.au,b.k.willcox@reading.ac.uk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -19249,6 +19320,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update folders for authors
</commit_message>
<xml_diff>
--- a/Datasets_Processing/Authors_Gdocs.xlsx
+++ b/Datasets_Processing/Authors_Gdocs.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="414">
   <si>
     <t xml:space="preserve">Study ID</t>
   </si>
@@ -397,10 +397,13 @@
     <t xml:space="preserve">veldtman@sun.ac.za</t>
   </si>
   <si>
-    <t xml:space="preserve">Ruan_Veldtman_Allium_cepa_South_Africa_2009</t>
+    <t xml:space="preserve">Mariette_Brand_Allium_cepa_South_Africa_2009</t>
   </si>
   <si>
     <t xml:space="preserve">Mariëtte R. Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruan_Veldtman_Allium_cepa_South_Africa_2009Mariette_Brand</t>
   </si>
   <si>
     <t xml:space="preserve">Ruan_Veldtman_Allium_cepa_South_Africa_2010</t>
@@ -1284,6 +1287,45 @@
   </si>
   <si>
     <t xml:space="preserve">Brad Howlett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silvia_Castro_Helianthus_annuus_Spain_2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sílvia Castro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scastro@bot.uc.pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucie Mota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">João Loureiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evan Marks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silvia_Castro_Helianthus_annuus_Spain_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silvia_Castro_Actinidia_deliciosa_Portugal_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helena Castro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hugo Gaspar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sílvia Castro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> João Loureiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silvia_Castro_Actinidia_deliciosa_Portugal_2019</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1336,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1400,6 +1442,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1472,7 +1526,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1625,6 +1679,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1704,13 +1766,13 @@
   </sheetPr>
   <dimension ref="A1:AA988"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A256" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E274" activeCellId="0" sqref="E274"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A274" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B290" activeCellId="0" sqref="B290"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.29"/>
@@ -5740,7 +5802,7 @@
       <c r="Z96" s="7"/>
       <c r="AA96" s="7"/>
     </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="8" t="s">
         <v>104</v>
       </c>
@@ -5754,7 +5816,7 @@
         <v>14</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F97" s="8"/>
       <c r="G97" s="9" t="n">
@@ -5785,9 +5847,9 @@
       <c r="Z97" s="7"/>
       <c r="AA97" s="7"/>
     </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>102</v>
@@ -5799,7 +5861,7 @@
         <v>103</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F98" s="8"/>
       <c r="G98" s="9"/>
@@ -5826,7 +5888,7 @@
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>105</v>
@@ -5871,7 +5933,7 @@
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>102</v>
@@ -5910,7 +5972,7 @@
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>102</v>
@@ -5919,7 +5981,7 @@
         <v>101</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>12</v>
@@ -5955,7 +6017,7 @@
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>100</v>
@@ -5994,16 +6056,16 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>12</v>
@@ -6039,10 +6101,10 @@
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>14</v>
@@ -6078,10 +6140,10 @@
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>14</v>
@@ -6117,10 +6179,10 @@
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>14</v>
@@ -6156,16 +6218,16 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>12</v>
@@ -6201,10 +6263,10 @@
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>14</v>
@@ -6240,10 +6302,10 @@
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>14</v>
@@ -6279,10 +6341,10 @@
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="B110" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>14</v>
@@ -6318,16 +6380,16 @@
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>12</v>
@@ -6363,16 +6425,16 @@
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>12</v>
@@ -6408,10 +6470,10 @@
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>14</v>
@@ -6447,16 +6509,16 @@
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>12</v>
@@ -6492,10 +6554,10 @@
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>14</v>
@@ -6531,16 +6593,16 @@
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>15</v>
@@ -6576,10 +6638,10 @@
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>14</v>
@@ -6615,16 +6677,16 @@
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>12</v>
@@ -6660,10 +6722,10 @@
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>14</v>
@@ -6699,16 +6761,16 @@
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>12</v>
@@ -6744,10 +6806,10 @@
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>14</v>
@@ -6783,7 +6845,7 @@
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>9</v>
@@ -6822,16 +6884,16 @@
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>12</v>
@@ -6867,16 +6929,16 @@
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C124" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D124" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C124" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D124" s="8" t="s">
-        <v>142</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>12</v>
@@ -6912,10 +6974,10 @@
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>14</v>
@@ -6951,16 +7013,16 @@
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>12</v>
@@ -6996,16 +7058,16 @@
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D127" s="13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>15</v>
@@ -7035,16 +7097,16 @@
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D128" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>15</v>
@@ -7074,16 +7136,16 @@
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>12</v>
@@ -7119,16 +7181,16 @@
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D130" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="B130" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D130" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="E130" s="5" t="s">
         <v>12</v>
@@ -7164,14 +7226,14 @@
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B131" s="5"/>
       <c r="C131" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D131" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>15</v>
@@ -7201,16 +7263,16 @@
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E132" s="8" t="s">
         <v>12</v>
@@ -7246,14 +7308,14 @@
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B133" s="8"/>
       <c r="C133" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D133" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E133" s="8" t="s">
         <v>15</v>
@@ -7283,16 +7345,16 @@
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>12</v>
@@ -7328,14 +7390,14 @@
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B135" s="5"/>
       <c r="C135" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D135" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>15</v>
@@ -7365,16 +7427,16 @@
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C136" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>12</v>
@@ -7410,14 +7472,14 @@
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B137" s="8"/>
       <c r="C137" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D137" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>15</v>
@@ -7447,16 +7509,16 @@
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>12</v>
@@ -7492,14 +7554,14 @@
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B139" s="5"/>
       <c r="C139" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D139" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>15</v>
@@ -7529,16 +7591,16 @@
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C140" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E140" s="8" t="s">
         <v>12</v>
@@ -7574,14 +7636,14 @@
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B141" s="8"/>
       <c r="C141" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D141" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E141" s="8" t="s">
         <v>15</v>
@@ -7611,16 +7673,16 @@
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>12</v>
@@ -7656,14 +7718,14 @@
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B143" s="5"/>
       <c r="C143" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D143" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>15</v>
@@ -7693,16 +7755,16 @@
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>12</v>
@@ -7738,16 +7800,16 @@
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D145" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="B145" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C145" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D145" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="E145" s="5" t="s">
         <v>12</v>
@@ -7783,16 +7845,16 @@
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E146" s="8" t="s">
         <v>12</v>
@@ -7828,16 +7890,16 @@
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C147" s="13" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E147" s="5" t="s">
         <v>12</v>
@@ -7873,16 +7935,16 @@
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C148" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>12</v>
@@ -7918,16 +7980,16 @@
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C149" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D149" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="B149" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C149" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="D149" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="E149" s="5" t="s">
         <v>12</v>
@@ -7963,16 +8025,16 @@
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C150" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E150" s="8" t="s">
         <v>12</v>
@@ -8008,16 +8070,16 @@
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E151" s="5" t="s">
         <v>12</v>
@@ -8053,16 +8115,16 @@
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C152" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E152" s="8" t="s">
         <v>12</v>
@@ -8098,13 +8160,13 @@
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C153" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D153" s="8" t="s">
         <v>14</v>
@@ -8137,13 +8199,13 @@
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D154" s="8" t="s">
         <v>14</v>
@@ -8176,13 +8238,13 @@
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B155" s="8" t="s">
         <v>73</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D155" s="8" t="s">
         <v>14</v>
@@ -8215,10 +8277,10 @@
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C156" s="5" t="s">
         <v>14</v>
@@ -8260,16 +8322,16 @@
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C157" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E157" s="5" t="s">
         <v>12</v>
@@ -8299,10 +8361,10 @@
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C158" s="8" t="s">
         <v>14</v>
@@ -8344,10 +8406,10 @@
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C159" s="8" t="s">
         <v>14</v>
@@ -8383,10 +8445,10 @@
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C160" s="8" t="s">
         <v>14</v>
@@ -8422,16 +8484,16 @@
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C161" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D161" s="8" t="s">
         <v>190</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D161" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>12</v>
@@ -8461,13 +8523,13 @@
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>14</v>
@@ -8506,16 +8568,16 @@
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C163" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E163" s="8" t="s">
         <v>12</v>
@@ -8551,13 +8613,13 @@
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C164" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D164" s="8" t="s">
         <v>14</v>
@@ -8590,16 +8652,16 @@
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E165" s="5" t="s">
         <v>12</v>
@@ -8635,16 +8697,16 @@
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C166" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D166" s="8" t="s">
         <v>204</v>
-      </c>
-      <c r="B166" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C166" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D166" s="8" t="s">
-        <v>203</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>12</v>
@@ -8680,16 +8742,16 @@
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D167" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E167" s="5" t="s">
         <v>15</v>
@@ -8725,16 +8787,16 @@
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C168" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="D168" s="20" t="s">
         <v>209</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C168" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="D168" s="20" t="s">
-        <v>208</v>
       </c>
       <c r="E168" s="8" t="s">
         <v>15</v>
@@ -8770,16 +8832,16 @@
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D169" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E169" s="5" t="s">
         <v>15</v>
@@ -8815,16 +8877,16 @@
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C170" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>12</v>
@@ -8860,10 +8922,10 @@
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C171" s="8" t="s">
         <v>14</v>
@@ -8899,10 +8961,10 @@
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C172" s="8" t="s">
         <v>14</v>
@@ -8938,16 +9000,16 @@
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E173" s="5" t="s">
         <v>12</v>
@@ -8983,13 +9045,13 @@
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>14</v>
@@ -9022,16 +9084,16 @@
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C175" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D175" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C175" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="D175" s="8" t="s">
-        <v>219</v>
       </c>
       <c r="E175" s="8" t="s">
         <v>12</v>
@@ -9067,13 +9129,13 @@
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C176" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D176" s="8" t="s">
         <v>14</v>
@@ -9106,13 +9168,13 @@
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D177" s="5" t="s">
         <v>14</v>
@@ -9151,10 +9213,10 @@
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C178" s="5" t="s">
         <v>14</v>
@@ -9190,13 +9252,13 @@
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C179" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D179" s="5" t="s">
         <v>14</v>
@@ -9229,16 +9291,16 @@
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>12</v>
@@ -9274,16 +9336,16 @@
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C181" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E181" s="5" t="s">
         <v>12</v>
@@ -9319,10 +9381,10 @@
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C182" s="5" t="s">
         <v>14</v>
@@ -9358,16 +9420,16 @@
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C183" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E183" s="8" t="s">
         <v>12</v>
@@ -9403,10 +9465,10 @@
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C184" s="8" t="s">
         <v>14</v>
@@ -9442,10 +9504,10 @@
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C185" s="8" t="s">
         <v>14</v>
@@ -9481,16 +9543,16 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C186" s="13" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E186" s="5" t="s">
         <v>12</v>
@@ -9526,16 +9588,16 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C187" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="D187" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="B187" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="C187" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="D187" s="8" t="s">
-        <v>239</v>
       </c>
       <c r="E187" s="8" t="s">
         <v>12</v>
@@ -9571,16 +9633,16 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C188" s="13" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E188" s="5" t="s">
         <v>12</v>
@@ -9616,16 +9678,16 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C189" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E189" s="8" t="s">
         <v>12</v>
@@ -9661,10 +9723,10 @@
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C190" s="8" t="s">
         <v>14</v>
@@ -9700,13 +9762,13 @@
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B191" s="17" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C191" s="17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D191" s="8" t="s">
         <v>14</v>
@@ -9739,16 +9801,16 @@
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C192" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D192" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E192" s="5" t="s">
         <v>12</v>
@@ -9784,16 +9846,16 @@
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C193" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D193" s="13" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E193" s="5" t="s">
         <v>15</v>
@@ -9823,16 +9885,16 @@
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C194" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>12</v>
@@ -9868,16 +9930,16 @@
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C195" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D195" s="8" t="s">
         <v>255</v>
-      </c>
-      <c r="B195" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="C195" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D195" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>12</v>
@@ -9913,16 +9975,16 @@
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C196" s="13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D196" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E196" s="5" t="s">
         <v>12</v>
@@ -9958,16 +10020,16 @@
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C197" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="D197" s="8" t="s">
         <v>260</v>
-      </c>
-      <c r="B197" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="C197" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="D197" s="8" t="s">
-        <v>259</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>12</v>
@@ -10003,16 +10065,16 @@
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C198" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D198" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E198" s="5" t="s">
         <v>12</v>
@@ -10048,16 +10110,16 @@
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C199" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D199" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="B199" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C199" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D199" s="8" t="s">
-        <v>263</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>12</v>
@@ -10093,16 +10155,16 @@
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C200" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D200" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E200" s="5" t="s">
         <v>12</v>
@@ -10138,16 +10200,16 @@
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C201" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D201" s="13" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E201" s="5" t="s">
         <v>15</v>
@@ -10177,16 +10239,16 @@
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C202" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E202" s="8" t="s">
         <v>12</v>
@@ -10222,16 +10284,16 @@
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C203" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D203" s="17" t="s">
         <v>270</v>
-      </c>
-      <c r="B203" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C203" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D203" s="17" t="s">
-        <v>269</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>15</v>
@@ -10261,16 +10323,16 @@
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D204" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="B204" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="C204" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D204" s="5" t="s">
-        <v>271</v>
       </c>
       <c r="E204" s="5" t="s">
         <v>12</v>
@@ -10306,16 +10368,16 @@
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C205" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D205" s="13" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E205" s="5" t="s">
         <v>15</v>
@@ -10345,16 +10407,16 @@
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C206" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E206" s="8" t="s">
         <v>12</v>
@@ -10390,10 +10452,10 @@
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C207" s="8" t="s">
         <v>14</v>
@@ -10429,10 +10491,10 @@
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C208" s="8" t="s">
         <v>14</v>
@@ -10468,10 +10530,10 @@
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C209" s="8" t="s">
         <v>14</v>
@@ -10507,10 +10569,10 @@
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C210" s="8" t="s">
         <v>14</v>
@@ -10546,10 +10608,10 @@
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C211" s="8" t="s">
         <v>14</v>
@@ -10585,10 +10647,10 @@
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C212" s="8" t="s">
         <v>14</v>
@@ -10624,10 +10686,10 @@
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C213" s="8" t="s">
         <v>14</v>
@@ -10663,16 +10725,16 @@
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D214" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E214" s="5" t="s">
         <v>15</v>
@@ -10708,7 +10770,7 @@
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B215" s="5" t="s">
         <v>83</v>
@@ -10747,16 +10809,16 @@
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C216" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D216" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E216" s="5" t="s">
         <v>12</v>
@@ -10786,16 +10848,16 @@
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C217" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D217" s="8" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E217" s="8" t="s">
         <v>12</v>
@@ -10831,10 +10893,10 @@
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C218" s="8" t="s">
         <v>14</v>
@@ -10870,16 +10932,16 @@
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C219" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D219" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E219" s="5" t="s">
         <v>12</v>
@@ -10915,16 +10977,16 @@
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="8" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C220" s="17" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D220" s="8" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E220" s="8" t="s">
         <v>12</v>
@@ -10960,16 +11022,16 @@
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C221" s="13" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D221" s="21" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E221" s="5" t="s">
         <v>12</v>
@@ -11005,13 +11067,13 @@
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C222" s="13" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D222" s="5" t="s">
         <v>14</v>
@@ -11044,7 +11106,7 @@
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B223" s="8" t="s">
         <v>17</v>
@@ -11053,7 +11115,7 @@
         <v>14</v>
       </c>
       <c r="D223" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E223" s="8" t="s">
         <v>12</v>
@@ -11089,7 +11151,7 @@
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B224" s="5" t="s">
         <v>17</v>
@@ -11098,7 +11160,7 @@
         <v>14</v>
       </c>
       <c r="D224" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E224" s="5" t="s">
         <v>12</v>
@@ -11134,16 +11196,16 @@
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C225" s="17" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D225" s="8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E225" s="8" t="s">
         <v>12</v>
@@ -11179,16 +11241,16 @@
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C226" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D226" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E226" s="5" t="s">
         <v>12</v>
@@ -11224,7 +11286,7 @@
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B227" s="5" t="s">
         <v>32</v>
@@ -11263,13 +11325,13 @@
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D228" s="5" t="s">
         <v>14</v>
@@ -11302,13 +11364,13 @@
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B229" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C229" s="13" t="s">
         <v>315</v>
-      </c>
-      <c r="C229" s="13" t="s">
-        <v>314</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>14</v>
@@ -11341,13 +11403,13 @@
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C230" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D230" s="5" t="s">
         <v>14</v>
@@ -11380,13 +11442,13 @@
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C231" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D231" s="5" t="s">
         <v>14</v>
@@ -11419,16 +11481,16 @@
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C232" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D232" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E232" s="8" t="s">
         <v>12</v>
@@ -11464,16 +11526,16 @@
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C233" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D233" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E233" s="5" t="s">
         <v>12</v>
@@ -11509,16 +11571,16 @@
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C234" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D234" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E234" s="8" t="s">
         <v>12</v>
@@ -11554,10 +11616,10 @@
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C235" s="8" t="s">
         <v>14</v>
@@ -11593,10 +11655,10 @@
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C236" s="8" t="s">
         <v>14</v>
@@ -11632,16 +11694,16 @@
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C237" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D237" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E237" s="5" t="s">
         <v>12</v>
@@ -11677,13 +11739,13 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B238" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D238" s="5" t="s">
         <v>98</v>
@@ -11716,16 +11778,16 @@
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D239" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E239" s="8" t="s">
         <v>12</v>
@@ -11761,13 +11823,13 @@
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D240" s="8" t="s">
         <v>14</v>
@@ -11800,16 +11862,16 @@
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C241" s="21" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D241" s="5" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E241" s="5" t="s">
         <v>12</v>
@@ -11845,16 +11907,16 @@
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D242" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E242" s="8" t="s">
         <v>12</v>
@@ -11890,16 +11952,16 @@
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C243" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D243" s="5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E243" s="5" t="s">
         <v>12</v>
@@ -11935,16 +11997,16 @@
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D244" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E244" s="8" t="s">
         <v>12</v>
@@ -11980,16 +12042,16 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="C245" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="D245" s="8" t="s">
         <v>349</v>
-      </c>
-      <c r="B245" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="C245" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="D245" s="8" t="s">
-        <v>348</v>
       </c>
       <c r="E245" s="8" t="s">
         <v>12</v>
@@ -12025,16 +12087,16 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C246" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D246" s="5" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E246" s="5" t="s">
         <v>12</v>
@@ -12070,16 +12132,16 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C247" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D247" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E247" s="8" t="s">
         <v>12</v>
@@ -12115,16 +12177,16 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C248" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D248" s="22" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E248" s="8" t="s">
         <v>15</v>
@@ -12154,16 +12216,16 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C249" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D249" s="5" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E249" s="5" t="s">
         <v>12</v>
@@ -12199,10 +12261,10 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C250" s="5" t="s">
         <v>14</v>
@@ -12238,16 +12300,16 @@
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C251" s="17" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D251" s="8" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E251" s="8" t="s">
         <v>12</v>
@@ -12283,16 +12345,16 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="5" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B252" s="13" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C252" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D252" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E252" s="5" t="s">
         <v>12</v>
@@ -12328,16 +12390,16 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B253" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C253" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D253" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E253" s="8" t="s">
         <v>12</v>
@@ -12373,13 +12435,13 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B254" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C254" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D254" s="8" t="s">
         <v>14</v>
@@ -12412,16 +12474,16 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C255" s="23" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D255" s="13" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E255" s="5" t="s">
         <v>12</v>
@@ -12457,10 +12519,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B256" s="13" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C256" s="23"/>
       <c r="D256" s="11"/>
@@ -12492,16 +12554,16 @@
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B257" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C257" s="24" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D257" s="17" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E257" s="8" t="s">
         <v>12</v>
@@ -12537,10 +12599,10 @@
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B258" s="12" t="s">
         <v>374</v>
-      </c>
-      <c r="B258" s="12" t="s">
-        <v>373</v>
       </c>
       <c r="C258" s="7"/>
       <c r="D258" s="7"/>
@@ -12572,14 +12634,14 @@
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B259" s="13" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C259" s="11"/>
       <c r="D259" s="13" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E259" s="5" t="s">
         <v>12</v>
@@ -12615,10 +12677,10 @@
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B260" s="25" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C260" s="11"/>
       <c r="D260" s="11"/>
@@ -12650,10 +12712,10 @@
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B261" s="13" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C261" s="11"/>
       <c r="D261" s="11"/>
@@ -12685,10 +12747,10 @@
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="7" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B262" s="16" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C262" s="7"/>
       <c r="D262" s="7"/>
@@ -12726,10 +12788,10 @@
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="7" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B263" s="27" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C263" s="7"/>
       <c r="D263" s="7"/>
@@ -12761,10 +12823,10 @@
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="7" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B264" s="27" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C264" s="7"/>
       <c r="D264" s="7"/>
@@ -12796,10 +12858,10 @@
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="5" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B265" s="13" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C265" s="11"/>
       <c r="D265" s="13"/>
@@ -12837,10 +12899,10 @@
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="5" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B266" s="25" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C266" s="11"/>
       <c r="D266" s="11"/>
@@ -12872,10 +12934,10 @@
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B267" s="13" t="s">
         <v>384</v>
-      </c>
-      <c r="B267" s="13" t="s">
-        <v>383</v>
       </c>
       <c r="C267" s="11"/>
       <c r="D267" s="11"/>
@@ -12907,14 +12969,14 @@
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B268" s="28" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C268" s="7"/>
       <c r="D268" s="16" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E268" s="7" t="s">
         <v>12</v>
@@ -12950,10 +13012,10 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B269" s="28" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C269" s="7"/>
       <c r="D269" s="7"/>
@@ -12985,10 +13047,10 @@
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B270" s="28" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C270" s="7"/>
       <c r="D270" s="7"/>
@@ -13016,10 +13078,10 @@
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="29" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B271" s="28" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C271" s="29"/>
       <c r="D271" s="29"/>
@@ -13051,14 +13113,14 @@
     </row>
     <row r="272" s="35" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="30" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B272" s="31" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C272" s="30"/>
       <c r="D272" s="32" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E272" s="33" t="s">
         <v>12</v>
@@ -13094,14 +13156,14 @@
     </row>
     <row r="273" s="35" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="30" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B273" s="36" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C273" s="30"/>
       <c r="D273" s="32" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E273" s="33" t="s">
         <v>15</v>
@@ -13131,14 +13193,14 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="29" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B274" s="16" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C274" s="29"/>
       <c r="D274" s="16" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E274" s="7" t="s">
         <v>12</v>
@@ -13174,10 +13236,10 @@
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="29" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B275" s="29" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C275" s="29"/>
       <c r="D275" s="29"/>
@@ -13209,10 +13271,10 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="29" t="s">
-        <v>396</v>
-      </c>
-      <c r="B276" s="37" t="s">
-        <v>398</v>
+        <v>397</v>
+      </c>
+      <c r="B276" s="29" t="s">
+        <v>399</v>
       </c>
       <c r="C276" s="29"/>
       <c r="D276" s="29"/>
@@ -13244,10 +13306,10 @@
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="29" t="s">
-        <v>396</v>
-      </c>
-      <c r="B277" s="37" t="s">
-        <v>399</v>
+        <v>397</v>
+      </c>
+      <c r="B277" s="29" t="s">
+        <v>400</v>
       </c>
       <c r="C277" s="29"/>
       <c r="D277" s="29"/>
@@ -13277,12 +13339,20 @@
       <c r="Z277" s="29"/>
       <c r="AA277" s="29"/>
     </row>
-    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="29"/>
-      <c r="B278" s="29"/>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="B278" s="16" t="s">
+        <v>402</v>
+      </c>
       <c r="C278" s="29"/>
-      <c r="D278" s="29"/>
-      <c r="E278" s="29"/>
+      <c r="D278" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="E278" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="F278" s="29"/>
       <c r="G278" s="29"/>
       <c r="H278" s="29"/>
@@ -13306,12 +13376,18 @@
       <c r="Z278" s="29"/>
       <c r="AA278" s="29"/>
     </row>
-    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="29"/>
-      <c r="B279" s="29"/>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="B279" s="37" t="s">
+        <v>404</v>
+      </c>
       <c r="C279" s="29"/>
       <c r="D279" s="29"/>
-      <c r="E279" s="29"/>
+      <c r="E279" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F279" s="29"/>
       <c r="G279" s="29"/>
       <c r="H279" s="29"/>
@@ -13335,12 +13411,18 @@
       <c r="Z279" s="29"/>
       <c r="AA279" s="29"/>
     </row>
-    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="29"/>
-      <c r="B280" s="29"/>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="B280" s="37" t="s">
+        <v>405</v>
+      </c>
       <c r="C280" s="29"/>
       <c r="D280" s="29"/>
-      <c r="E280" s="29"/>
+      <c r="E280" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F280" s="29"/>
       <c r="G280" s="29"/>
       <c r="H280" s="29"/>
@@ -13364,12 +13446,18 @@
       <c r="Z280" s="29"/>
       <c r="AA280" s="29"/>
     </row>
-    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="29"/>
-      <c r="B281" s="29"/>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="B281" s="37" t="s">
+        <v>406</v>
+      </c>
       <c r="C281" s="29"/>
       <c r="D281" s="29"/>
-      <c r="E281" s="29"/>
+      <c r="E281" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F281" s="29"/>
       <c r="G281" s="29"/>
       <c r="H281" s="29"/>
@@ -13393,12 +13481,20 @@
       <c r="Z281" s="29"/>
       <c r="AA281" s="29"/>
     </row>
-    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="29"/>
-      <c r="B282" s="29"/>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="B282" s="16" t="s">
+        <v>402</v>
+      </c>
       <c r="C282" s="29"/>
-      <c r="D282" s="29"/>
-      <c r="E282" s="29"/>
+      <c r="D282" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="E282" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="F282" s="29"/>
       <c r="G282" s="29"/>
       <c r="H282" s="29"/>
@@ -13422,12 +13518,18 @@
       <c r="Z282" s="29"/>
       <c r="AA282" s="29"/>
     </row>
-    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="29"/>
-      <c r="B283" s="29"/>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="37" t="s">
+        <v>407</v>
+      </c>
+      <c r="B283" s="37" t="s">
+        <v>404</v>
+      </c>
       <c r="C283" s="29"/>
       <c r="D283" s="29"/>
-      <c r="E283" s="29"/>
+      <c r="E283" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F283" s="29"/>
       <c r="G283" s="29"/>
       <c r="H283" s="29"/>
@@ -13451,12 +13553,18 @@
       <c r="Z283" s="29"/>
       <c r="AA283" s="29"/>
     </row>
-    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="29"/>
-      <c r="B284" s="29"/>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="37" t="s">
+        <v>407</v>
+      </c>
+      <c r="B284" s="37" t="s">
+        <v>405</v>
+      </c>
       <c r="C284" s="29"/>
       <c r="D284" s="29"/>
-      <c r="E284" s="29"/>
+      <c r="E284" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F284" s="29"/>
       <c r="G284" s="29"/>
       <c r="H284" s="29"/>
@@ -13480,12 +13588,18 @@
       <c r="Z284" s="29"/>
       <c r="AA284" s="29"/>
     </row>
-    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="29"/>
-      <c r="B285" s="29"/>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="37" t="s">
+        <v>407</v>
+      </c>
+      <c r="B285" s="37" t="s">
+        <v>406</v>
+      </c>
       <c r="C285" s="29"/>
       <c r="D285" s="29"/>
-      <c r="E285" s="29"/>
+      <c r="E285" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F285" s="29"/>
       <c r="G285" s="29"/>
       <c r="H285" s="29"/>
@@ -13509,12 +13623,18 @@
       <c r="Z285" s="29"/>
       <c r="AA285" s="29"/>
     </row>
-    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="29"/>
-      <c r="B286" s="29"/>
+    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="B286" s="38" t="s">
+        <v>409</v>
+      </c>
       <c r="C286" s="29"/>
       <c r="D286" s="29"/>
-      <c r="E286" s="29"/>
+      <c r="E286" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F286" s="29"/>
       <c r="G286" s="29"/>
       <c r="H286" s="29"/>
@@ -13538,12 +13658,18 @@
       <c r="Z286" s="29"/>
       <c r="AA286" s="29"/>
     </row>
-    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="29"/>
-      <c r="B287" s="29"/>
+    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="B287" s="38" t="s">
+        <v>410</v>
+      </c>
       <c r="C287" s="29"/>
       <c r="D287" s="29"/>
-      <c r="E287" s="29"/>
+      <c r="E287" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F287" s="29"/>
       <c r="G287" s="29"/>
       <c r="H287" s="29"/>
@@ -13567,12 +13693,20 @@
       <c r="Z287" s="29"/>
       <c r="AA287" s="29"/>
     </row>
-    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="29"/>
-      <c r="B288" s="29"/>
+    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="B288" s="38" t="s">
+        <v>411</v>
+      </c>
       <c r="C288" s="29"/>
-      <c r="D288" s="29"/>
-      <c r="E288" s="29"/>
+      <c r="D288" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="E288" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="F288" s="29"/>
       <c r="G288" s="29"/>
       <c r="H288" s="29"/>
@@ -13596,12 +13730,18 @@
       <c r="Z288" s="29"/>
       <c r="AA288" s="29"/>
     </row>
-    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="29"/>
-      <c r="B289" s="29"/>
+    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="B289" s="38" t="s">
+        <v>412</v>
+      </c>
       <c r="C289" s="29"/>
       <c r="D289" s="29"/>
-      <c r="E289" s="29"/>
+      <c r="E289" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F289" s="29"/>
       <c r="G289" s="29"/>
       <c r="H289" s="29"/>
@@ -13625,12 +13765,18 @@
       <c r="Z289" s="29"/>
       <c r="AA289" s="29"/>
     </row>
-    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="29"/>
-      <c r="B290" s="29"/>
+    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="29" t="s">
+        <v>413</v>
+      </c>
+      <c r="B290" s="38" t="s">
+        <v>409</v>
+      </c>
       <c r="C290" s="29"/>
       <c r="D290" s="29"/>
-      <c r="E290" s="29"/>
+      <c r="E290" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F290" s="29"/>
       <c r="G290" s="29"/>
       <c r="H290" s="29"/>
@@ -13654,12 +13800,18 @@
       <c r="Z290" s="29"/>
       <c r="AA290" s="29"/>
     </row>
-    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="29"/>
-      <c r="B291" s="29"/>
+    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="39" t="s">
+        <v>413</v>
+      </c>
+      <c r="B291" s="38" t="s">
+        <v>410</v>
+      </c>
       <c r="C291" s="29"/>
       <c r="D291" s="29"/>
-      <c r="E291" s="29"/>
+      <c r="E291" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F291" s="29"/>
       <c r="G291" s="29"/>
       <c r="H291" s="29"/>
@@ -13683,20 +13835,34 @@
       <c r="Z291" s="29"/>
       <c r="AA291" s="29"/>
     </row>
-    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="27"/>
-      <c r="B292" s="27"/>
+    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="39" t="s">
+        <v>413</v>
+      </c>
+      <c r="B292" s="38" t="s">
+        <v>411</v>
+      </c>
       <c r="C292" s="27"/>
-      <c r="D292" s="27"/>
-      <c r="E292" s="27"/>
+      <c r="D292" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="E292" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="F292" s="27"/>
     </row>
-    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="27"/>
-      <c r="B293" s="27"/>
+    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="39" t="s">
+        <v>413</v>
+      </c>
+      <c r="B293" s="38" t="s">
+        <v>412</v>
+      </c>
       <c r="C293" s="27"/>
       <c r="D293" s="27"/>
-      <c r="E293" s="27"/>
+      <c r="E293" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F293" s="27"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>